<commit_message>
Update Student Job Application Webview and other
</commit_message>
<xml_diff>
--- a/highedin/student_service/Workflow.xlsx
+++ b/highedin/student_service/Workflow.xlsx
@@ -365,12 +365,107 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Document Type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Is Active</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Don't Override Status</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Send Email Alert</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Workflow State Field</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>ID (Document States)</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>State (Document States)</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Doc Status (Document States)</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Update Field (Document States)</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Update Value (Document States)</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Is Optional State (Document States)</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Next Action Email Template (Document States)</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Only Allow Edit For (Document States)</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Message (Document States)</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
         <is>
           <t>ID (Transitions)</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>State (Transitions)</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Action (Transitions)</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Next State (Transitions)</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Allowed (Transitions)</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Allow Self Approval (Transitions)</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Condition (Transitions)</t>
         </is>
       </c>
     </row>
@@ -382,62 +477,339 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Student Leave Request</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>workflow_state</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>f8238d66bc</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Draft</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
         <is>
           <t>7265fb9bd1</t>
         </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Draft</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Send to Instructor</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="U2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
         <is>
           <t>cbf6b64242</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
         <is>
           <t>a75892c2ee</t>
         </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Send to Instructor</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+      <c r="U3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
         <is>
           <t>4f137fc4f8</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Approved</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
         <is>
           <t>a303542dbc</t>
         </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Approve</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Approved</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+      <c r="U4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
         <is>
           <t>6e7e9072ca</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Rejected</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
         <is>
           <t>23da67e03f</t>
         </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Rejected</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Reject</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Rejected</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+      <c r="U5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
         <is>
           <t>758cf7be7b</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -447,97 +819,525 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>Student General Request</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>workflow_state</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>1e2089589b</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Draft</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
         <is>
           <t>7653419ca8</t>
         </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Draft</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Send to Instructor</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="U7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr">
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
         <is>
           <t>8bfa67244d</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
         <is>
           <t>5dd997469f</t>
         </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Send to Staff</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Sending</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+      <c r="U8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr">
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
         <is>
           <t>4d9f2c2638</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Rejected</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
         <is>
           <t>fd2dcffdb0</t>
         </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Reject</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Rejected</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+      <c r="U9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
         <is>
           <t>c31e06c1f7</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Sending</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
         <is>
           <t>93f91ebb4b</t>
         </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Sending</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Send to Dean</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Deciding</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Staff</t>
+        </is>
+      </c>
+      <c r="U10" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
         <is>
           <t>8bd95b37ed</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Deciding</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Dean</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Dean</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
         <is>
           <t>e2f627e351</t>
         </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Deciding</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Approve</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Approved</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Dean</t>
+        </is>
+      </c>
+      <c r="U11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
         <is>
           <t>41cb0b7a58</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Approved</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Dean</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
         <is>
           <t>c7fec9c33e</t>
         </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Deciding</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Reject</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Rejected</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>Dean</t>
+        </is>
+      </c>
+      <c r="U12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
         <is>
           <t>f33adb57bd</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Rejected</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Dean</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
         <is>
           <t>2c706af929</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>send_to</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>